<commit_message>
Latest executables and some bug fixes
</commit_message>
<xml_diff>
--- a/Entrance_Gate_ECU/TestCases/Entrance-Gate_ECU_TestCases.xlsx
+++ b/Entrance_Gate_ECU/TestCases/Entrance-Gate_ECU_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn-In-Depth\Private_Vechicle_Parking\Entrance_Gate_ECU\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8901D8-7E66-40A6-BA24-1EA23DB438CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEF4B64-4612-4396-8FA0-FB4D362CBACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
   <si>
     <t>Test ID</t>
   </si>
@@ -154,6 +154,129 @@
   </si>
   <si>
     <t>Functional Test</t>
+  </si>
+  <si>
+    <t>Validate the 
+functionality of
+sending the ID
+to the Admin ECU</t>
+  </si>
+  <si>
+    <t>Send_0</t>
+  </si>
+  <si>
+    <t>Test that we are 
+able to send the 
+ID to the main ECU</t>
+  </si>
+  <si>
+    <t>1.Microship Studio
+2.Proteus
+3.GPIO Driver
+4.SPI Driver
+5.Main ECU Drivers</t>
+  </si>
+  <si>
+    <t>ID  = "000"</t>
+  </si>
+  <si>
+    <t>Main ECU received
+the ID</t>
+  </si>
+  <si>
+    <t>Send_1</t>
+  </si>
+  <si>
+    <t>Test that we don't 
+get stuck in this
+phase if anything 
+fails</t>
+  </si>
+  <si>
+    <t>Return to the
+welcome message
+screen</t>
+  </si>
+  <si>
+    <t>1.Microship Studio
+2.Proteus
+3.GPIO Driver
+4.SPI Driver
+5.Timer0 Driver
+6.Main ECU Drivers</t>
+  </si>
+  <si>
+    <t>Test that we are 
+able to validate an
+authorized ID</t>
+  </si>
+  <si>
+    <t>Validate the
+functionality of
+receiving the 
+authentication 
+process Result</t>
+  </si>
+  <si>
+    <t>Auth_ID0</t>
+  </si>
+  <si>
+    <t>Validate the 
+functionality of
+reading the driver ID</t>
+  </si>
+  <si>
+    <t>ReadID_0</t>
+  </si>
+  <si>
+    <t>Test that we can read the 3 digits ID successfully</t>
+  </si>
+  <si>
+    <t>1.Microship Studio
+2.Proteus
+3.GPIO Driver
+4.LCD HAL Driver
+5.UART Driver</t>
+  </si>
+  <si>
+    <t>ID = "000"</t>
+  </si>
+  <si>
+    <t>"000" printed on the terminal</t>
+  </si>
+  <si>
+    <t>ReadID_1</t>
+  </si>
+  <si>
+    <t>Test that we can’t input more than 3 digits</t>
+  </si>
+  <si>
+    <t>ID = "0000"</t>
+  </si>
+  <si>
+    <t>"000" printed on the terminal and the uart is disabled</t>
+  </si>
+  <si>
+    <t>ID ="000"
+IDS_LIST = {"000"}</t>
+  </si>
+  <si>
+    <t>Prints "Valid ID" on the LCD</t>
+  </si>
+  <si>
+    <t>Auth_ID1</t>
+  </si>
+  <si>
+    <t>Test that we are 
+able to reject an
+unauthorized ID</t>
+  </si>
+  <si>
+    <t>ID ="111"
+IDS_LIST = {"000"}</t>
+  </si>
+  <si>
+    <t>Prints "Invalid ID" on the LCD</t>
   </si>
 </sst>
 </file>
@@ -183,7 +306,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,8 +331,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -241,11 +370,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -253,23 +391,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -664,220 +823,453 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+    <row r="3" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="I3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="4" t="s">
+      <c r="I5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="4" t="s">
+      <c r="I6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="4" t="s">
+      <c r="I8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:K1">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
@@ -895,7 +1287,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
     <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
-      <formula>$H$40</formula>
+      <formula>$H$43</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>